<commit_message>
dev-mapping: added vis of connections by distance
</commit_message>
<xml_diff>
--- a/GasGrid/PopulatingTools/Mapping and Location Tools/location.xlsx
+++ b/GasGrid/PopulatingTools/Mapping and Location Tools/location.xlsx
@@ -190,7 +190,7 @@
     <t>57.57062000000001</t>
   </si>
   <si>
-    <t>53.2446664</t>
+    <t>53.2414752</t>
   </si>
   <si>
     <t>54.5435025</t>
@@ -265,7 +265,7 @@
     <t>-1.83803</t>
   </si>
   <si>
-    <t>-2.4370474</t>
+    <t>-2.4474069</t>
   </si>
   <si>
     <t>-1.3301732</t>
@@ -508,7 +508,7 @@
     <t xml:space="preserve"> Fordoun</t>
   </si>
   <si>
-    <t xml:space="preserve"> GooleGlass</t>
+    <t xml:space="preserve"> Goole</t>
   </si>
   <si>
     <t xml:space="preserve"> ICI Billnghm</t>
@@ -526,7 +526,7 @@
     <t xml:space="preserve"> Conoco Philips Teeside</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rough</t>
+    <t>Easington</t>
   </si>
   <si>
     <t xml:space="preserve">St Fergus </t>
@@ -565,7 +565,7 @@
     <t>56.876579</t>
   </si>
   <si>
-    <t>52.5124167</t>
+    <t>53.702941</t>
   </si>
   <si>
     <t>54.612537</t>
@@ -583,7 +583,7 @@
     <t>54.61630299999999</t>
   </si>
   <si>
-    <t>51.5211024</t>
+    <t>54.783504</t>
   </si>
   <si>
     <t>56.0962295</t>
@@ -619,7 +619,7 @@
     <t>-2.412157</t>
   </si>
   <si>
-    <t>-2.0403782</t>
+    <t>-0.876381</t>
   </si>
   <si>
     <t>-1.290961</t>
@@ -637,7 +637,7 @@
     <t>-1.170778</t>
   </si>
   <si>
-    <t>-0.07249259999999999</t>
+    <t>-1.3516487</t>
   </si>
   <si>
     <t>-3.3098061</t>
@@ -655,7 +655,7 @@
     <t xml:space="preserve"> Alrewas</t>
   </si>
   <si>
-    <t xml:space="preserve"> Armadale</t>
+    <t xml:space="preserve"> Armadale West Lothian</t>
   </si>
   <si>
     <t xml:space="preserve"> Aspley</t>
@@ -991,10 +991,10 @@
     <t xml:space="preserve"> Winkfield</t>
   </si>
   <si>
-    <t xml:space="preserve"> Yelverton</t>
-  </si>
-  <si>
-    <t>57.064863</t>
+    <t xml:space="preserve"> Yelverton Norwich</t>
+  </si>
+  <si>
+    <t>55.897742</t>
   </si>
   <si>
     <t>52.97204079999999</t>
@@ -1015,7 +1015,7 @@
     <t>54.205613</t>
   </si>
   <si>
-    <t>55.7845661</t>
+    <t>56.4783817</t>
   </si>
   <si>
     <t>55.9024</t>
@@ -1297,10 +1297,10 @@
     <t>51.4420486</t>
   </si>
   <si>
-    <t>50.493452</t>
-  </si>
-  <si>
-    <t>-5.901249</t>
+    <t>52.5745368</t>
+  </si>
+  <si>
+    <t>-3.702162</t>
   </si>
   <si>
     <t>-1.200032</t>
@@ -1321,7 +1321,7 @@
     <t>-1.452231</t>
   </si>
   <si>
-    <t>-4.3703994</t>
+    <t>-2.9748214</t>
   </si>
   <si>
     <t>-3.643118</t>
@@ -1603,7 +1603,7 @@
     <t>-0.6975153</t>
   </si>
   <si>
-    <t>-4.085603</t>
+    <t>1.3804957</t>
   </si>
   <si>
     <t>Power Station</t>

</xml_diff>